<commit_message>
Added ld reservoir lat/long.  Created site map
</commit_message>
<xml_diff>
--- a/ohio2016/inputData/LouisDistReservoirHydrology.xlsx
+++ b/ohio2016/inputData/LouisDistReservoirHydrology.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Aa.ad.epa.gov\ord\CIN\Users\main\F-K\JBEAULIE\Net MyDocuments\Documents\research\EPA\East Fork Reservoir\ACE\multiResSurvey\ohio\inputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JBEAULIE\GitRepository\mulitResSurvey\ohio2016\inputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,6 +617,9 @@
       </c>
       <c r="D8">
         <v>5</v>
+      </c>
+      <c r="E8">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>